<commit_message>
allow xlsx column header variance for First or First Name
</commit_message>
<xml_diff>
--- a/testdata/USWNT.CurrentRoster.xlsx
+++ b/testdata/USWNT.CurrentRoster.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danhi/Documents/GitHub/Projects/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A7A66E1-B5CF-254E-B895-954A730C7425}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FC50A78-6E80-D34F-A3FE-282D0113402D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="880" yWindow="1460" windowWidth="24640" windowHeight="14000" xr2:uid="{8C3BE1C5-2F3F-8840-AA91-AE07AF3D1B90}"/>
   </bookViews>
@@ -345,12 +345,6 @@
     <t>Press</t>
   </si>
   <si>
-    <t>First Name</t>
-  </si>
-  <si>
-    <t>Last Name</t>
-  </si>
-  <si>
     <t>Lloyd </t>
   </si>
   <si>
@@ -376,6 +370,12 @@
   </si>
   <si>
     <t>Rebecca</t>
+  </si>
+  <si>
+    <t>First</t>
+  </si>
+  <si>
+    <t>Last</t>
   </si>
 </sst>
 </file>
@@ -739,7 +739,7 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:J7"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -764,10 +764,10 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="E1" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
@@ -782,7 +782,7 @@
         <v>6</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -883,7 +883,7 @@
         <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E5" t="s">
         <v>68</v>
@@ -988,7 +988,7 @@
         <v>55</v>
       </c>
       <c r="J8" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -1020,7 +1020,7 @@
         <v>54</v>
       </c>
       <c r="J9" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
@@ -1052,7 +1052,7 @@
         <v>56</v>
       </c>
       <c r="J10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
@@ -1084,7 +1084,7 @@
         <v>58</v>
       </c>
       <c r="J11" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
@@ -1116,7 +1116,7 @@
         <v>58</v>
       </c>
       <c r="J12" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
@@ -1148,7 +1148,7 @@
         <v>54</v>
       </c>
       <c r="J13" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
@@ -1180,7 +1180,7 @@
         <v>54</v>
       </c>
       <c r="J14" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
@@ -1212,7 +1212,7 @@
         <v>56</v>
       </c>
       <c r="J15" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
@@ -1244,7 +1244,7 @@
         <v>59</v>
       </c>
       <c r="J16" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
@@ -1276,7 +1276,7 @@
         <v>60</v>
       </c>
       <c r="J17" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
@@ -1308,7 +1308,7 @@
         <v>59</v>
       </c>
       <c r="J18" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
@@ -1319,13 +1319,13 @@
         <v>42</v>
       </c>
       <c r="C19" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D19" t="s">
         <v>95</v>
       </c>
       <c r="E19" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F19" t="s">
         <v>45</v>
@@ -1340,7 +1340,7 @@
         <v>61</v>
       </c>
       <c r="J19" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
@@ -1351,13 +1351,13 @@
         <v>42</v>
       </c>
       <c r="C20" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D20" t="s">
         <v>96</v>
       </c>
       <c r="E20" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F20" t="s">
         <v>46</v>
@@ -1372,7 +1372,7 @@
         <v>55</v>
       </c>
       <c r="J20" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
@@ -1383,13 +1383,13 @@
         <v>42</v>
       </c>
       <c r="C21" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D21" t="s">
         <v>97</v>
       </c>
       <c r="E21" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F21" t="s">
         <v>47</v>
@@ -1404,7 +1404,7 @@
         <v>60</v>
       </c>
       <c r="J21" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
@@ -1436,7 +1436,7 @@
         <v>56</v>
       </c>
       <c r="J22" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
@@ -1468,7 +1468,7 @@
         <v>58</v>
       </c>
       <c r="J23" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
@@ -1500,7 +1500,7 @@
         <v>57</v>
       </c>
       <c r="J24" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>